<commit_message>
pretty GUI up bsed on feedback
</commit_message>
<xml_diff>
--- a/notes/shop costs.xlsx
+++ b/notes/shop costs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="225">
   <si>
     <t>Item</t>
   </si>
@@ -560,9 +560,6 @@
   </si>
   <si>
     <t>steam turbine</t>
-  </si>
-  <si>
-    <t>hull component</t>
   </si>
   <si>
     <t>Habitation</t>
@@ -1162,11 +1159,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q109"/>
+  <dimension ref="A1:Q108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1207,7 +1204,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1227,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E78" si="0">SUM(B2+10+C2)/D2</f>
+        <f t="shared" ref="E2:E77" si="0">SUM(B2+10+C2)/D2</f>
         <v>13.5</v>
       </c>
       <c r="F2">
@@ -2631,26 +2628,26 @@
       <c r="O59" s="3"/>
       <c r="Q59" s="3"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75">
+    <row r="60" spans="1:17" ht="18" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B60">
-        <f>(F25)*2500+(F6)*1000</f>
-        <v>3258500</v>
+        <f>(F4)*5+(F2)*10</f>
+        <v>280</v>
       </c>
       <c r="C60" s="3">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D60" s="3">
         <v>1</v>
       </c>
       <c r="E60">
         <f t="shared" si="0"/>
-        <v>3258560</v>
+        <v>298</v>
       </c>
       <c r="F60">
-        <v>3258560</v>
+        <v>298</v>
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="5"/>
@@ -2659,13 +2656,13 @@
       <c r="O60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="61" spans="1:17" ht="18" customHeight="1">
+    <row r="61" spans="1:17" ht="12.75">
       <c r="A61" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B61">
-        <f>(F4)*5+(F2)*10</f>
-        <v>280</v>
+        <f>(F60)*7+(F42)*5+(F6)*5</f>
+        <v>3251</v>
       </c>
       <c r="C61" s="3">
         <v>8</v>
@@ -2675,10 +2672,10 @@
       </c>
       <c r="E61">
         <f t="shared" si="0"/>
-        <v>298</v>
+        <v>3269</v>
       </c>
       <c r="F61">
-        <v>298</v>
+        <v>3269</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="5"/>
@@ -2689,24 +2686,24 @@
     </row>
     <row r="62" spans="1:17" ht="12.75">
       <c r="A62" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B62">
-        <f>(F61)*7+(F42)*5+(F6)*5</f>
-        <v>3251</v>
+        <f>F4+F7+F10</f>
+        <v>194</v>
       </c>
       <c r="C62" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D62" s="3">
         <v>1</v>
       </c>
       <c r="E62">
         <f t="shared" si="0"/>
-        <v>3269</v>
+        <v>205</v>
       </c>
       <c r="F62">
-        <v>3269</v>
+        <v>205</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="5"/>
@@ -2720,8 +2717,8 @@
         <v>176</v>
       </c>
       <c r="B63">
-        <f>F4+F7+F10</f>
-        <v>194</v>
+        <f>F3*5</f>
+        <v>210</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
@@ -2731,10 +2728,10 @@
       </c>
       <c r="E63">
         <f t="shared" si="0"/>
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="F63">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="G63" s="17"/>
       <c r="H63" s="5"/>
@@ -2745,24 +2742,24 @@
     </row>
     <row r="64" spans="1:17" ht="12.75">
       <c r="A64" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B64">
-        <f>F3*5</f>
-        <v>210</v>
+        <f>F6+F2+(F4)</f>
+        <v>208</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
       </c>
       <c r="D64" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64">
         <f t="shared" si="0"/>
-        <v>221</v>
+        <v>109.5</v>
       </c>
       <c r="F64">
-        <v>221</v>
+        <v>110</v>
       </c>
       <c r="G64" s="17"/>
       <c r="H64" s="5"/>
@@ -2776,21 +2773,21 @@
         <v>179</v>
       </c>
       <c r="B65">
-        <f>F6+F2+(F4)</f>
-        <v>208</v>
+        <f>(F7)*5+(F10)*3+(F4)*10</f>
+        <v>912</v>
       </c>
       <c r="C65" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65">
         <f t="shared" si="0"/>
-        <v>109.5</v>
+        <v>924</v>
       </c>
       <c r="F65">
-        <v>110</v>
+        <v>924</v>
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="5"/>
@@ -2801,24 +2798,24 @@
     </row>
     <row r="66" spans="1:17" ht="12.75">
       <c r="A66" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B66">
-        <f>(F7)*5+(F10)*3+(F4)*10</f>
-        <v>912</v>
+        <f>(F10)*3+(F7)*5+(F4)*9</f>
+        <v>884</v>
       </c>
       <c r="C66" s="3">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D66" s="3">
         <v>1</v>
       </c>
       <c r="E66">
         <f t="shared" si="0"/>
-        <v>924</v>
+        <v>894.5</v>
       </c>
       <c r="F66">
-        <v>924</v>
+        <v>895</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="5"/>
@@ -2832,8 +2829,8 @@
         <v>182</v>
       </c>
       <c r="B67">
-        <f>(F10)*3+(F7)*5+(F4)*9</f>
-        <v>884</v>
+        <f>(F6)*2+(F10)*3+(F7)*5+(F66)</f>
+        <v>1859</v>
       </c>
       <c r="C67" s="3">
         <v>0.5</v>
@@ -2843,10 +2840,10 @@
       </c>
       <c r="E67">
         <f t="shared" si="0"/>
-        <v>894.5</v>
+        <v>1869.5</v>
       </c>
       <c r="F67">
-        <v>895</v>
+        <v>1870</v>
       </c>
       <c r="G67" s="17"/>
       <c r="H67" s="5"/>
@@ -2857,24 +2854,24 @@
     </row>
     <row r="68" spans="1:17" ht="12.75">
       <c r="A68" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B68">
-        <f>(F6)*2+(F10)*3+(F7)*5+(F67)</f>
-        <v>1859</v>
+        <f>(F6)*15+(F7)*10+(F3)*10+(F10)*10+(F11)*10</f>
+        <v>4960</v>
       </c>
       <c r="C68" s="3">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="D68" s="3">
         <v>1</v>
       </c>
       <c r="E68">
         <f t="shared" si="0"/>
-        <v>1869.5</v>
+        <v>4978</v>
       </c>
       <c r="F68">
-        <v>1870</v>
+        <v>4978</v>
       </c>
       <c r="G68" s="17"/>
       <c r="H68" s="5"/>
@@ -2885,24 +2882,24 @@
     </row>
     <row r="69" spans="1:17" ht="12.75">
       <c r="A69" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B69">
-        <f>(F6)*15+(F7)*10+(F3)*10+(F10)*10+(F11)*10</f>
-        <v>4960</v>
+        <f>(F23*5) + (F6*10) + (F3*10)</f>
+        <v>4180</v>
       </c>
       <c r="C69" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D69" s="3">
         <v>1</v>
       </c>
       <c r="E69">
         <f t="shared" si="0"/>
-        <v>4978</v>
+        <v>4195</v>
       </c>
       <c r="F69">
-        <v>4978</v>
+        <v>4195</v>
       </c>
       <c r="G69" s="17"/>
       <c r="H69" s="5"/>
@@ -2916,8 +2913,8 @@
         <v>192</v>
       </c>
       <c r="B70">
-        <f>(F23*5) + (F6*10) + (F3*10)</f>
-        <v>4180</v>
+        <f>F5 + F7</f>
+        <v>95</v>
       </c>
       <c r="C70" s="3">
         <v>5</v>
@@ -2927,10 +2924,10 @@
       </c>
       <c r="E70">
         <f t="shared" si="0"/>
-        <v>4195</v>
+        <v>110</v>
       </c>
       <c r="F70">
-        <v>4195</v>
+        <v>110</v>
       </c>
       <c r="G70" s="17"/>
       <c r="H70" s="5"/>
@@ -2944,21 +2941,21 @@
         <v>193</v>
       </c>
       <c r="B71">
-        <f>F5 + F7</f>
-        <v>95</v>
+        <f>F8 + F62</f>
+        <v>258</v>
       </c>
       <c r="C71" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D71" s="3">
         <v>1</v>
       </c>
       <c r="E71">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>274</v>
       </c>
       <c r="F71">
-        <v>110</v>
+        <v>274</v>
       </c>
       <c r="G71" s="17"/>
       <c r="H71" s="5"/>
@@ -2972,21 +2969,21 @@
         <v>194</v>
       </c>
       <c r="B72">
-        <f>F8 + F63</f>
-        <v>258</v>
+        <f>F60+F40+(F63*2)</f>
+        <v>1182</v>
       </c>
       <c r="C72" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D72" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E72">
         <f t="shared" si="0"/>
-        <v>274</v>
+        <v>601</v>
       </c>
       <c r="F72">
-        <v>274</v>
+        <v>601</v>
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="5"/>
@@ -2997,24 +2994,24 @@
     </row>
     <row r="73" spans="1:17" ht="12.75">
       <c r="A73" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B73">
-        <f>F61+F40+(F64*2)</f>
-        <v>1182</v>
+        <f>(F23*3) + (F26*2) + F28</f>
+        <v>1984</v>
       </c>
       <c r="C73" s="3">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D73" s="3">
         <v>2</v>
       </c>
       <c r="E73">
         <f t="shared" si="0"/>
-        <v>601</v>
+        <v>1009</v>
       </c>
       <c r="F73">
-        <v>601</v>
+        <v>1009</v>
       </c>
       <c r="G73" s="17"/>
       <c r="H73" s="5"/>
@@ -3028,21 +3025,21 @@
         <v>198</v>
       </c>
       <c r="B74">
-        <f>(F23*3) + (F26*2) + F28</f>
-        <v>1984</v>
+        <f>F33+F69+(F64*30)</f>
+        <v>10115</v>
       </c>
       <c r="C74" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D74" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E74">
         <f t="shared" si="0"/>
-        <v>1009</v>
+        <v>3382</v>
       </c>
       <c r="F74">
-        <v>1009</v>
+        <v>3382</v>
       </c>
       <c r="G74" s="17"/>
       <c r="H74" s="5"/>
@@ -3053,11 +3050,11 @@
     </row>
     <row r="75" spans="1:17" ht="12.75">
       <c r="A75" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B75">
-        <f>F33+F70+(F65*30)</f>
-        <v>10115</v>
+        <f>F32+(F25*3)+(F24*2)</f>
+        <v>11328</v>
       </c>
       <c r="C75" s="3">
         <v>21</v>
@@ -3067,10 +3064,10 @@
       </c>
       <c r="E75">
         <f t="shared" si="0"/>
-        <v>3382</v>
+        <v>3786.3333333333335</v>
       </c>
       <c r="F75">
-        <v>3382</v>
+        <v>3787</v>
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="5"/>
@@ -3083,78 +3080,56 @@
       <c r="A76" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B76">
-        <f>F32+(F25*3)+(F24*2)</f>
-        <v>11328</v>
+      <c r="B76" s="17">
+        <f>F38+F55</f>
+        <v>8040285</v>
       </c>
       <c r="C76" s="3">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D76" s="3">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="E76">
         <f t="shared" si="0"/>
-        <v>3786.3333333333335</v>
+        <v>8040.3549999999996</v>
       </c>
       <c r="F76">
-        <v>3787</v>
+        <v>8041</v>
       </c>
       <c r="G76" s="17"/>
       <c r="H76" s="5"/>
       <c r="J76" s="3"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="3"/>
-      <c r="Q76" s="3"/>
     </row>
     <row r="77" spans="1:17" ht="12.75">
       <c r="A77" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B77" s="17">
-        <f>F38+F55</f>
-        <v>8040285</v>
+        <v>203</v>
+      </c>
+      <c r="B77">
+        <f>SUM(F70:F76)</f>
+        <v>17204</v>
       </c>
       <c r="C77" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D77" s="3">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="E77">
         <f t="shared" si="0"/>
-        <v>8040.3549999999996</v>
+        <v>17214</v>
       </c>
       <c r="F77">
-        <v>8041</v>
-      </c>
-      <c r="G77" s="17"/>
-      <c r="H77" s="5"/>
+        <v>17214</v>
+      </c>
+      <c r="G77" s="5"/>
+      <c r="H77" s="17"/>
       <c r="J77" s="3"/>
     </row>
     <row r="78" spans="1:17" ht="12.75">
-      <c r="A78" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B78">
-        <f>SUM(F71:F77)</f>
-        <v>17204</v>
-      </c>
-      <c r="C78" s="3">
-        <v>0</v>
-      </c>
-      <c r="D78" s="3">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <f t="shared" si="0"/>
-        <v>17214</v>
-      </c>
-      <c r="F78">
-        <v>17214</v>
-      </c>
-      <c r="G78" s="5"/>
-      <c r="H78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="5"/>
       <c r="J78" s="3"/>
     </row>
     <row r="79" spans="1:17" ht="12.75">
@@ -3163,35 +3138,40 @@
       <c r="H79" s="5"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:17" ht="12.75">
+    <row r="80" spans="1:17" ht="14.25">
+      <c r="A80" s="20"/>
       <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="17"/>
       <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="N80" s="16"/>
+      <c r="O80" s="16"/>
     </row>
     <row r="81" spans="1:15" ht="14.25">
       <c r="A81" s="20"/>
       <c r="F81" s="17"/>
       <c r="G81" s="5"/>
       <c r="H81" s="17"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
       <c r="N81" s="16"/>
       <c r="O81" s="16"/>
     </row>
     <row r="82" spans="1:15" ht="14.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="20" t="s">
+        <v>224</v>
+      </c>
       <c r="F82" s="17"/>
       <c r="G82" s="5"/>
       <c r="H82" s="17"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
       <c r="N82" s="16"/>
       <c r="O82" s="16"/>
     </row>
     <row r="83" spans="1:15" ht="14.25">
-      <c r="A83" s="20" t="s">
-        <v>225</v>
-      </c>
+      <c r="A83" s="20"/>
       <c r="F83" s="17"/>
       <c r="G83" s="5"/>
       <c r="H83" s="17"/>
@@ -3206,9 +3186,6 @@
       <c r="F84" s="17"/>
       <c r="G84" s="5"/>
       <c r="H84" s="17"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
       <c r="N84" s="16"/>
       <c r="O84" s="16"/>
     </row>
@@ -3217,6 +3194,9 @@
       <c r="F85" s="17"/>
       <c r="G85" s="5"/>
       <c r="H85" s="17"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
       <c r="N85" s="16"/>
       <c r="O85" s="16"/>
     </row>
@@ -3225,9 +3205,6 @@
       <c r="F86" s="17"/>
       <c r="G86" s="5"/>
       <c r="H86" s="17"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
       <c r="N86" s="16"/>
       <c r="O86" s="16"/>
     </row>
@@ -3255,116 +3232,138 @@
       <c r="N89" s="16"/>
       <c r="O89" s="16"/>
     </row>
-    <row r="90" spans="1:15" ht="14.25">
-      <c r="A90" s="20"/>
+    <row r="90" spans="1:15" ht="12.75">
       <c r="F90" s="17"/>
-      <c r="G90" s="5"/>
+      <c r="G90" s="17"/>
       <c r="H90" s="17"/>
-      <c r="N90" s="16"/>
-      <c r="O90" s="16"/>
-    </row>
-    <row r="91" spans="1:15" ht="12.75">
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
+    </row>
+    <row r="91" spans="1:15" ht="15">
+      <c r="A91" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B91">
+        <f>(F6*50)+(F23*30)</f>
+        <v>20900</v>
+      </c>
+      <c r="C91" s="3">
+        <v>15</v>
+      </c>
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <f t="shared" ref="E91:E108" si="1">SUM(B91+10+C91)/D91</f>
+        <v>20925</v>
+      </c>
+      <c r="F91" s="17">
+        <v>20925</v>
+      </c>
+      <c r="G91" s="5">
+        <f>F91/100</f>
+        <v>209.25</v>
+      </c>
+      <c r="H91" s="17">
+        <f t="shared" ref="H91:H92" si="2">IF(G91 &lt; 1000, ROUND(G91,-1), IF(G91 &lt; 10000, ROUND(G91,-2), ROUND(G91,-3)))</f>
+        <v>210</v>
+      </c>
     </row>
     <row r="92" spans="1:15" ht="15">
       <c r="A92" s="22" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B92">
-        <f>(F6*50)+(F23*30)</f>
-        <v>20900</v>
+        <f>(F6*40)+(F24*40)+(F27*20)</f>
+        <v>135920</v>
       </c>
       <c r="C92" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D92" s="3">
         <v>1</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92:E109" si="1">SUM(B92+10+C92)/D92</f>
-        <v>20925</v>
+        <f t="shared" si="1"/>
+        <v>135950</v>
       </c>
       <c r="F92" s="17">
-        <v>20925</v>
+        <v>135950</v>
       </c>
       <c r="G92" s="5">
-        <f>F92/100</f>
-        <v>209.25</v>
+        <f t="shared" ref="G92:G108" si="3">F92/100</f>
+        <v>1359.5</v>
       </c>
       <c r="H92" s="17">
-        <f t="shared" ref="H92:H93" si="2">IF(G92 &lt; 1000, ROUND(G92,-1), IF(G92 &lt; 10000, ROUND(G92,-2), ROUND(G92,-3)))</f>
-        <v>210</v>
+        <f t="shared" si="2"/>
+        <v>1400</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="15">
       <c r="A93" s="22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B93">
-        <f>(F6*40)+(F24*40)+(F27*20)</f>
-        <v>135920</v>
+        <f>SUM(F34*50)+(F24*60)+(F27*40)+(F25*30)</f>
+        <v>1594820</v>
       </c>
       <c r="C93" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D93" s="3">
         <v>1</v>
       </c>
       <c r="E93">
         <f t="shared" si="1"/>
-        <v>135950</v>
+        <v>1594855</v>
       </c>
       <c r="F93" s="17">
-        <v>135950</v>
+        <v>1594855</v>
       </c>
       <c r="G93" s="5">
-        <f t="shared" ref="G93:G109" si="3">F93/100</f>
-        <v>1359.5</v>
+        <f t="shared" si="3"/>
+        <v>15948.55</v>
       </c>
       <c r="H93" s="17">
-        <f t="shared" si="2"/>
-        <v>1400</v>
+        <f>IF(G93 &lt; 1000, ROUND(G93,-1), IF(G93 &lt; 10000, ROUND(G93,-2), ROUND(G93,-3)))</f>
+        <v>16000</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="15">
       <c r="A94" s="22" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B94">
-        <f>SUM(F34*50)+(F24*60)+(F27*40)+(F25*30)</f>
-        <v>1594820</v>
+        <f>(F6*5)+(F23*2)+F30</f>
+        <v>4145</v>
       </c>
       <c r="C94" s="3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D94" s="3">
         <v>1</v>
       </c>
       <c r="E94">
         <f t="shared" si="1"/>
-        <v>1594855</v>
+        <v>4165</v>
       </c>
       <c r="F94" s="17">
-        <v>1594855</v>
+        <v>4165</v>
       </c>
       <c r="G94" s="5">
         <f t="shared" si="3"/>
-        <v>15948.55</v>
+        <v>41.65</v>
       </c>
       <c r="H94" s="17">
-        <f>IF(G94 &lt; 1000, ROUND(G94,-1), IF(G94 &lt; 10000, ROUND(G94,-2), ROUND(G94,-3)))</f>
-        <v>16000</v>
+        <f t="shared" ref="H94:H96" si="4">IF(G94 &lt; 1000, ROUND(G94,-1), IF(G94 &lt; 10000, ROUND(G94,-2), ROUND(G94,-3)))</f>
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="15">
       <c r="A95" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B95">
-        <f>(F6*5)+(F23*2)+F30</f>
-        <v>4145</v>
+        <f>(F24*200)+(50*F25)</f>
+        <v>642850</v>
       </c>
       <c r="C95" s="3">
         <v>10</v>
@@ -3374,18 +3373,18 @@
       </c>
       <c r="E95">
         <f t="shared" si="1"/>
-        <v>4165</v>
+        <v>642870</v>
       </c>
       <c r="F95" s="17">
-        <v>4165</v>
+        <v>642870</v>
       </c>
       <c r="G95" s="5">
         <f t="shared" si="3"/>
-        <v>41.65</v>
+        <v>6428.7</v>
       </c>
       <c r="H95" s="17">
-        <f t="shared" ref="H95:H109" si="4">IF(G95 &lt; 1000, ROUND(G95,-1), IF(G95 &lt; 10000, ROUND(G95,-2), ROUND(G95,-3)))</f>
-        <v>40</v>
+        <f t="shared" si="4"/>
+        <v>6400</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="15">
@@ -3393,8 +3392,8 @@
         <v>205</v>
       </c>
       <c r="B96">
-        <f>(F24*200)+(50*F25)</f>
-        <v>642850</v>
+        <f>(F6*10)+(F23*5)</f>
+        <v>3760</v>
       </c>
       <c r="C96" s="3">
         <v>10</v>
@@ -3404,18 +3403,18 @@
       </c>
       <c r="E96">
         <f t="shared" si="1"/>
-        <v>642870</v>
+        <v>3780</v>
       </c>
       <c r="F96" s="17">
-        <v>642870</v>
+        <v>3780</v>
       </c>
       <c r="G96" s="5">
         <f t="shared" si="3"/>
-        <v>6428.7</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="H96" s="17">
         <f t="shared" si="4"/>
-        <v>6400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15">
@@ -3423,8 +3422,8 @@
         <v>206</v>
       </c>
       <c r="B97">
-        <f>(F6*10)+(F23*5)</f>
-        <v>3760</v>
+        <f>(F96*10)+(5*F24)+(F25*5)</f>
+        <v>58510</v>
       </c>
       <c r="C97" s="3">
         <v>10</v>
@@ -3434,18 +3433,18 @@
       </c>
       <c r="E97">
         <f t="shared" si="1"/>
-        <v>3780</v>
+        <v>58530</v>
       </c>
       <c r="F97" s="17">
-        <v>3780</v>
+        <v>58530</v>
       </c>
       <c r="G97" s="5">
         <f t="shared" si="3"/>
-        <v>37.799999999999997</v>
+        <v>585.29999999999995</v>
       </c>
       <c r="H97" s="17">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f>IF(G97 &lt; 1000, ROUND(G97,-1), IF(G97 &lt; 10000, ROUND(G97,-2), ROUND(G97,-3)))</f>
+        <v>590</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15">
@@ -3453,8 +3452,8 @@
         <v>207</v>
       </c>
       <c r="B98">
-        <f>(F97*10)+(5*F24)+(F25*5)</f>
-        <v>58510</v>
+        <f>(F6*10)+(F19*5)</f>
+        <v>3310</v>
       </c>
       <c r="C98" s="3">
         <v>10</v>
@@ -3464,27 +3463,27 @@
       </c>
       <c r="E98">
         <f t="shared" si="1"/>
-        <v>58530</v>
+        <v>3330</v>
       </c>
       <c r="F98" s="17">
-        <v>58530</v>
+        <v>3330</v>
       </c>
       <c r="G98" s="5">
         <f t="shared" si="3"/>
-        <v>585.29999999999995</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="H98" s="17">
-        <f>IF(G98 &lt; 1000, ROUND(G98,-1), IF(G98 &lt; 10000, ROUND(G98,-2), ROUND(G98,-3)))</f>
-        <v>590</v>
+        <f t="shared" ref="H98:H108" si="5">IF(G98 &lt; 1000, ROUND(G98,-1), IF(G98 &lt; 10000, ROUND(G98,-2), ROUND(G98,-3)))</f>
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15">
       <c r="A99" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B99">
-        <f>(F6*10)+(F19*5)</f>
-        <v>3310</v>
+        <f>(F98*10)+(F24*15)+(F25*5)</f>
+        <v>83060</v>
       </c>
       <c r="C99" s="3">
         <v>10</v>
@@ -3494,27 +3493,27 @@
       </c>
       <c r="E99">
         <f t="shared" si="1"/>
-        <v>3330</v>
+        <v>83080</v>
       </c>
       <c r="F99" s="17">
-        <v>3330</v>
+        <v>83080</v>
       </c>
       <c r="G99" s="5">
         <f t="shared" si="3"/>
-        <v>33.299999999999997</v>
+        <v>830.8</v>
       </c>
       <c r="H99" s="17">
-        <f t="shared" ref="H99:H109" si="5">IF(G99 &lt; 1000, ROUND(G99,-1), IF(G99 &lt; 10000, ROUND(G99,-2), ROUND(G99,-3)))</f>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>830</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15">
       <c r="A100" s="22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B100">
-        <f>(F99*10)+(F24*15)+(F25*5)</f>
-        <v>83060</v>
+        <f>(F24*20)+(F25*5)+(F31*5)</f>
+        <v>110735</v>
       </c>
       <c r="C100" s="3">
         <v>10</v>
@@ -3524,27 +3523,27 @@
       </c>
       <c r="E100">
         <f t="shared" si="1"/>
-        <v>83080</v>
+        <v>110755</v>
       </c>
       <c r="F100" s="17">
-        <v>83080</v>
+        <v>110755</v>
       </c>
       <c r="G100" s="5">
         <f t="shared" si="3"/>
-        <v>830.8</v>
+        <v>1107.55</v>
       </c>
       <c r="H100" s="17">
         <f t="shared" si="5"/>
-        <v>830</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15">
       <c r="A101" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B101">
-        <f>(F24*20)+(F25*5)+(F31*5)</f>
-        <v>110735</v>
+        <f>(F6*20)+(F24*10)+(F27*30)</f>
+        <v>51990</v>
       </c>
       <c r="C101" s="3">
         <v>10</v>
@@ -3554,18 +3553,18 @@
       </c>
       <c r="E101">
         <f t="shared" si="1"/>
-        <v>110755</v>
+        <v>52010</v>
       </c>
       <c r="F101" s="17">
-        <v>110755</v>
+        <v>52010</v>
       </c>
       <c r="G101" s="5">
         <f t="shared" si="3"/>
-        <v>1107.55</v>
+        <v>520.1</v>
       </c>
       <c r="H101" s="17">
         <f t="shared" si="5"/>
-        <v>1100</v>
+        <v>520</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15">
@@ -3573,8 +3572,8 @@
         <v>216</v>
       </c>
       <c r="B102">
-        <f>(F6*20)+(F24*10)+(F27*30)</f>
-        <v>51990</v>
+        <f>SUM(F19*45)+(F7*40)+(F6*20)+(F23*10)</f>
+        <v>25050</v>
       </c>
       <c r="C102" s="3">
         <v>10</v>
@@ -3584,18 +3583,18 @@
       </c>
       <c r="E102">
         <f t="shared" si="1"/>
-        <v>52010</v>
+        <v>25070</v>
       </c>
       <c r="F102" s="17">
-        <v>52010</v>
+        <v>25070</v>
       </c>
       <c r="G102" s="5">
         <f t="shared" si="3"/>
-        <v>520.1</v>
+        <v>250.7</v>
       </c>
       <c r="H102" s="17">
         <f t="shared" si="5"/>
-        <v>520</v>
+        <v>250</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="15">
@@ -3603,29 +3602,29 @@
         <v>217</v>
       </c>
       <c r="B103">
-        <f>SUM(F19*45)+(F7*40)+(F6*20)+(F23*10)</f>
-        <v>25050</v>
+        <f>(100*F24)+(20*F25)+(F102*5)</f>
+        <v>440590</v>
       </c>
       <c r="C103" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
       </c>
       <c r="E103">
         <f t="shared" si="1"/>
-        <v>25070</v>
+        <v>440620</v>
       </c>
       <c r="F103" s="17">
-        <v>25070</v>
+        <v>440620</v>
       </c>
       <c r="G103" s="5">
         <f t="shared" si="3"/>
-        <v>250.7</v>
+        <v>4406.2</v>
       </c>
       <c r="H103" s="17">
         <f t="shared" si="5"/>
-        <v>250</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="15">
@@ -3633,37 +3632,37 @@
         <v>218</v>
       </c>
       <c r="B104">
-        <f>(100*F24)+(20*F25)+(F103*5)</f>
-        <v>440590</v>
+        <f>(F6*10)+(F23*5)</f>
+        <v>3760</v>
       </c>
       <c r="C104" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D104" s="3">
         <v>1</v>
       </c>
       <c r="E104">
         <f t="shared" si="1"/>
-        <v>440620</v>
+        <v>3780</v>
       </c>
       <c r="F104" s="17">
-        <v>440620</v>
+        <v>3780</v>
       </c>
       <c r="G104" s="5">
         <f t="shared" si="3"/>
-        <v>4406.2</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="H104" s="17">
         <f t="shared" si="5"/>
-        <v>4400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="15">
       <c r="A105" s="22" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B105">
-        <f>(F6*10)+(F23*5)</f>
+        <f>(10*F6) + (5*F23)</f>
         <v>3760</v>
       </c>
       <c r="C105" s="3">
@@ -3690,41 +3689,41 @@
     </row>
     <row r="106" spans="1:8" ht="15">
       <c r="A106" s="22" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B106">
-        <f>(10*F6) + (5*F23)</f>
-        <v>3760</v>
+        <f>F32+(F10*2)</f>
+        <v>2005</v>
       </c>
       <c r="C106" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
       </c>
       <c r="E106">
         <f t="shared" si="1"/>
-        <v>3780</v>
+        <v>2016</v>
       </c>
       <c r="F106" s="17">
-        <v>3780</v>
+        <v>2016</v>
       </c>
       <c r="G106" s="5">
         <f t="shared" si="3"/>
-        <v>37.799999999999997</v>
+        <v>20.16</v>
       </c>
       <c r="H106" s="17">
         <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="15">
-      <c r="A107" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="12.75">
+      <c r="A107" s="3" t="s">
         <v>220</v>
       </c>
       <c r="B107">
-        <f>F32+(F10*2)</f>
-        <v>2005</v>
+        <f>SUM(F12+(F10*3)+F23)</f>
+        <v>2056</v>
       </c>
       <c r="C107" s="3">
         <v>1</v>
@@ -3734,14 +3733,14 @@
       </c>
       <c r="E107">
         <f t="shared" si="1"/>
-        <v>2016</v>
+        <v>2067</v>
       </c>
       <c r="F107" s="17">
-        <v>2016</v>
+        <v>2067</v>
       </c>
       <c r="G107" s="5">
         <f t="shared" si="3"/>
-        <v>20.16</v>
+        <v>20.67</v>
       </c>
       <c r="H107" s="17">
         <f t="shared" si="5"/>
@@ -3753,57 +3752,27 @@
         <v>221</v>
       </c>
       <c r="B108">
-        <f>SUM(F12+(F10*3)+F23)</f>
-        <v>2056</v>
+        <f>SUM(F6*45)+(F7*45)+(F23*45)</f>
+        <v>29385</v>
       </c>
       <c r="C108" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
       </c>
       <c r="E108">
         <f t="shared" si="1"/>
-        <v>2067</v>
+        <v>29400</v>
       </c>
       <c r="F108" s="17">
-        <v>2067</v>
+        <v>29400</v>
       </c>
       <c r="G108" s="5">
         <f t="shared" si="3"/>
-        <v>20.67</v>
+        <v>294</v>
       </c>
       <c r="H108" s="17">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="12.75">
-      <c r="A109" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B109">
-        <f>SUM(F6*45)+(F7*45)+(F23*45)</f>
-        <v>29385</v>
-      </c>
-      <c r="C109" s="3">
-        <v>5</v>
-      </c>
-      <c r="D109" s="3">
-        <v>1</v>
-      </c>
-      <c r="E109">
-        <f t="shared" si="1"/>
-        <v>29400</v>
-      </c>
-      <c r="F109" s="17">
-        <v>29400</v>
-      </c>
-      <c r="G109" s="5">
-        <f t="shared" si="3"/>
-        <v>294</v>
-      </c>
-      <c r="H109" s="17">
         <f t="shared" si="5"/>
         <v>290</v>
       </c>
@@ -5292,7 +5261,7 @@
     </row>
     <row r="40" spans="1:24" ht="14.25">
       <c r="A40" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40">
         <f>SUM(G6*100)+(G20*500)+(100*G22)+(G23*100)</f>
@@ -5348,7 +5317,7 @@
     </row>
     <row r="41" spans="1:24" ht="14.25">
       <c r="A41" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B41">
         <f>SUM(100*G22)+(G23*100)+(G11*200)+(50*G33)</f>
@@ -5392,7 +5361,7 @@
     </row>
     <row r="42" spans="1:24" ht="28.5">
       <c r="A42" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B42">
         <f>SUM(200*G20)+(100*G22)+(G23*100)+(G33*150)</f>
@@ -5436,7 +5405,7 @@
     </row>
     <row r="43" spans="1:24" ht="14.25">
       <c r="A43" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B43">
         <f>SUM(300*G22)+(G23*100)+(G33*50)</f>
@@ -5478,12 +5447,12 @@
         <v>1.9781946809572761E-2</v>
       </c>
       <c r="X43" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="28.5">
       <c r="A44" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B44">
         <f>SUM(G22*500)+(G23*100)+(G33*1500)</f>
@@ -5513,10 +5482,10 @@
         <v>2236700</v>
       </c>
       <c r="J44" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="P44" s="16">
         <f t="shared" si="8"/>
@@ -5531,7 +5500,7 @@
         <v>7.429174820065775E-4</v>
       </c>
       <c r="X44" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="12.75">
@@ -5542,13 +5511,13 @@
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
       <c r="M45" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N45" s="18"/>
     </row>
     <row r="46" spans="1:24" ht="15">
       <c r="A46" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46">
         <f>(G6*50)+(G21*30)</f>
@@ -5587,12 +5556,12 @@
         <v>15000</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="15">
       <c r="A47" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B47">
         <f>(G6*40)+(G22*40)+(G25*20)</f>
@@ -5637,7 +5606,7 @@
     </row>
     <row r="48" spans="1:24" ht="15">
       <c r="A48" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B48">
         <f>SUM(G32*50)+(G22*60)+(G25*40)+(G23*30)</f>
@@ -5679,7 +5648,7 @@
     </row>
     <row r="49" spans="1:21" ht="15">
       <c r="A49" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B49">
         <f>(G6*5)+(G21*2)+G28</f>
@@ -5721,7 +5690,7 @@
     </row>
     <row r="50" spans="1:21" ht="15">
       <c r="A50" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50">
         <f>(G22*200)+(50*G23)</f>
@@ -5763,7 +5732,7 @@
     </row>
     <row r="51" spans="1:21" ht="15">
       <c r="A51" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B51">
         <f>(G6*10)+(G21*5)</f>
@@ -5798,7 +5767,7 @@
     </row>
     <row r="52" spans="1:21" ht="15">
       <c r="A52" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52">
         <f>(G51*10)+(5*G22)+(G23*5)</f>
@@ -5842,7 +5811,7 @@
     </row>
     <row r="53" spans="1:21" ht="15">
       <c r="A53" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B53">
         <f>(G6*10)+(G18*5)</f>
@@ -5872,12 +5841,12 @@
         <v>40</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="15">
       <c r="A54" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B54">
         <f>(G53*10)+(G22*15)+(G23*5)</f>
@@ -5911,18 +5880,18 @@
         <v>47580</v>
       </c>
       <c r="S54" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T54" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="T54" s="3" t="s">
+      <c r="U54" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="U54" s="3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="15">
       <c r="A55" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55">
         <f>(G22*20)+(G23*5)+(G29*5)</f>
@@ -5952,7 +5921,7 @@
         <v>1150</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T55" s="23">
         <v>2000000</v>
@@ -5963,7 +5932,7 @@
     </row>
     <row r="56" spans="1:21" ht="15">
       <c r="A56" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B56">
         <f>(G6*20)+(G22*10)+(G25*30)</f>
@@ -6006,7 +5975,7 @@
     </row>
     <row r="57" spans="1:21" ht="15">
       <c r="A57" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B57">
         <f>SUM(G18*45)+(G7*40)+(G6*20)+(G21*10)</f>
@@ -6049,7 +6018,7 @@
     </row>
     <row r="58" spans="1:21" ht="15">
       <c r="A58" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B58">
         <f>(100*G22)+(20*G23)+(G57*5)</f>
@@ -6092,7 +6061,7 @@
     </row>
     <row r="59" spans="1:21" ht="15">
       <c r="A59" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B59">
         <f>(G6*10)+(G21*5)</f>
@@ -6135,7 +6104,7 @@
     </row>
     <row r="60" spans="1:21" ht="15">
       <c r="A60" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B60">
         <f>G30+(G10*2)</f>
@@ -6188,7 +6157,7 @@
     </row>
     <row r="62" spans="1:21" ht="12.75">
       <c r="A62" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B62">
         <f>SUM(G12+(G10*3)+G21)</f>
@@ -6227,7 +6196,7 @@
     </row>
     <row r="63" spans="1:21" ht="12.75">
       <c r="A63" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B63">
         <f>SUM(G6*45)+(G7*45)+(G21*45)</f>

</xml_diff>